<commit_message>
Updated workbook. Added 50 charts.
</commit_message>
<xml_diff>
--- a/data-in-workbook.xlsx
+++ b/data-in-workbook.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -444,7 +444,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -623,11 +622,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1424982944"/>
-        <c:axId val="1296751120"/>
+        <c:axId val="1421416032"/>
+        <c:axId val="1421419424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1424982944"/>
+        <c:axId val="1421416032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -673,7 +672,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -739,12 +737,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1296751120"/>
+        <c:crossAx val="1421419424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1296751120"/>
+        <c:axId val="1421419424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -800,7 +798,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1424982944"/>
+        <c:crossAx val="1421416032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -864,7 +862,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1043,11 +1040,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1442226256"/>
-        <c:axId val="1440407856"/>
+        <c:axId val="1173393744"/>
+        <c:axId val="1173397136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1442226256"/>
+        <c:axId val="1173393744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1093,7 +1090,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1159,12 +1155,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440407856"/>
+        <c:crossAx val="1173397136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1440407856"/>
+        <c:axId val="1173397136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1220,7 +1216,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1442226256"/>
+        <c:crossAx val="1173393744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1284,7 +1280,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1463,11 +1458,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1029895504"/>
-        <c:axId val="1030622896"/>
+        <c:axId val="1436479792"/>
+        <c:axId val="1173405648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1029895504"/>
+        <c:axId val="1436479792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1513,7 +1508,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1579,12 +1573,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1030622896"/>
+        <c:crossAx val="1173405648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1030622896"/>
+        <c:axId val="1173405648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,7 +1634,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1029895504"/>
+        <c:crossAx val="1436479792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1704,7 +1698,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1883,11 +1876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1425484096"/>
-        <c:axId val="1029880160"/>
+        <c:axId val="1173426176"/>
+        <c:axId val="1173430208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1425484096"/>
+        <c:axId val="1173426176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1933,7 +1926,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1999,12 +1991,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1029880160"/>
+        <c:crossAx val="1173430208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1029880160"/>
+        <c:axId val="1173430208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2060,7 +2052,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1425484096"/>
+        <c:crossAx val="1173426176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2124,7 +2116,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2303,11 +2294,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1425920640"/>
-        <c:axId val="1425267712"/>
+        <c:axId val="1173450464"/>
+        <c:axId val="1173454496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1425920640"/>
+        <c:axId val="1173450464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2353,7 +2344,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2419,12 +2409,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1425267712"/>
+        <c:crossAx val="1173454496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1425267712"/>
+        <c:axId val="1173454496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2480,7 +2470,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1425920640"/>
+        <c:crossAx val="1173450464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2544,7 +2534,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2723,11 +2712,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1029805456"/>
-        <c:axId val="1030054032"/>
+        <c:axId val="1173475104"/>
+        <c:axId val="1173479136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1029805456"/>
+        <c:axId val="1173475104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2773,7 +2762,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2839,12 +2827,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1030054032"/>
+        <c:crossAx val="1173479136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1030054032"/>
+        <c:axId val="1173479136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2900,7 +2888,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1029805456"/>
+        <c:crossAx val="1173475104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2964,7 +2952,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3143,11 +3130,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1425923968"/>
-        <c:axId val="1030282128"/>
+        <c:axId val="1173497584"/>
+        <c:axId val="1173501616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1425923968"/>
+        <c:axId val="1173497584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3193,7 +3180,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3259,12 +3245,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1030282128"/>
+        <c:crossAx val="1173501616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1030282128"/>
+        <c:axId val="1173501616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3320,7 +3306,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1425923968"/>
+        <c:crossAx val="1173497584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3384,7 +3370,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3563,11 +3548,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1425038592"/>
-        <c:axId val="1030627216"/>
+        <c:axId val="1173519824"/>
+        <c:axId val="1173523856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1425038592"/>
+        <c:axId val="1173519824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3613,7 +3598,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3679,12 +3663,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1030627216"/>
+        <c:crossAx val="1173523856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1030627216"/>
+        <c:axId val="1173523856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3740,7 +3724,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1425038592"/>
+        <c:crossAx val="1173519824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3804,7 +3788,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3983,11 +3966,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1425400800"/>
-        <c:axId val="1029840256"/>
+        <c:axId val="1173544384"/>
+        <c:axId val="1173548416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1425400800"/>
+        <c:axId val="1173544384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4033,7 +4016,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4099,12 +4081,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1029840256"/>
+        <c:crossAx val="1173548416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1029840256"/>
+        <c:axId val="1173548416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4160,7 +4142,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1425400800"/>
+        <c:crossAx val="1173544384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4224,7 +4206,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4403,11 +4384,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1425973536"/>
-        <c:axId val="1421137440"/>
+        <c:axId val="1173569376"/>
+        <c:axId val="1173573408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1425973536"/>
+        <c:axId val="1173569376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4453,7 +4434,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4519,12 +4499,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1421137440"/>
+        <c:crossAx val="1173573408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1421137440"/>
+        <c:axId val="1173573408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4580,7 +4560,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1425973536"/>
+        <c:crossAx val="1173569376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4644,7 +4624,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4823,11 +4802,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1425926464"/>
-        <c:axId val="1029849296"/>
+        <c:axId val="1396878544"/>
+        <c:axId val="1397238432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1425926464"/>
+        <c:axId val="1396878544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4873,7 +4852,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4939,12 +4917,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1029849296"/>
+        <c:crossAx val="1397238432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1029849296"/>
+        <c:axId val="1397238432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5000,7 +4978,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1425926464"/>
+        <c:crossAx val="1396878544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5064,7 +5042,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5243,11 +5220,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1400792208"/>
-        <c:axId val="1440434304"/>
+        <c:axId val="1420826368"/>
+        <c:axId val="1420829760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1400792208"/>
+        <c:axId val="1420826368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5293,7 +5270,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5359,12 +5335,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440434304"/>
+        <c:crossAx val="1420829760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1440434304"/>
+        <c:axId val="1420829760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5420,7 +5396,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1400792208"/>
+        <c:crossAx val="1420826368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5484,7 +5460,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5663,11 +5638,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1425633760"/>
-        <c:axId val="1425636880"/>
+        <c:axId val="1171776320"/>
+        <c:axId val="1396931376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1425633760"/>
+        <c:axId val="1171776320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5713,7 +5688,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5779,12 +5753,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1425636880"/>
+        <c:crossAx val="1396931376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1425636880"/>
+        <c:axId val="1396931376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5840,7 +5814,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1425633760"/>
+        <c:crossAx val="1171776320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5904,7 +5878,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6083,11 +6056,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1027657360"/>
-        <c:axId val="1298012016"/>
+        <c:axId val="1397500592"/>
+        <c:axId val="1397324624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1027657360"/>
+        <c:axId val="1397500592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6133,7 +6106,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6199,12 +6171,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1298012016"/>
+        <c:crossAx val="1397324624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1298012016"/>
+        <c:axId val="1397324624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6260,7 +6232,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1027657360"/>
+        <c:crossAx val="1397500592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6324,7 +6296,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6503,11 +6474,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1090709280"/>
-        <c:axId val="1027651312"/>
+        <c:axId val="1397141712"/>
+        <c:axId val="1397160224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1090709280"/>
+        <c:axId val="1397141712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6553,7 +6524,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6619,12 +6589,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1027651312"/>
+        <c:crossAx val="1397160224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1027651312"/>
+        <c:axId val="1397160224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6680,7 +6650,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1090709280"/>
+        <c:crossAx val="1397141712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6744,7 +6714,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6923,11 +6892,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1090714464"/>
-        <c:axId val="1090570464"/>
+        <c:axId val="1397272848"/>
+        <c:axId val="1397379776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1090714464"/>
+        <c:axId val="1397272848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6973,7 +6942,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7039,12 +7007,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1090570464"/>
+        <c:crossAx val="1397379776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1090570464"/>
+        <c:axId val="1397379776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7100,7 +7068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1090714464"/>
+        <c:crossAx val="1397272848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7164,7 +7132,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7343,11 +7310,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1090786496"/>
-        <c:axId val="1090905040"/>
+        <c:axId val="1171682832"/>
+        <c:axId val="1397570752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1090786496"/>
+        <c:axId val="1171682832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7393,7 +7360,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7459,12 +7425,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1090905040"/>
+        <c:crossAx val="1397570752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1090905040"/>
+        <c:axId val="1397570752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7520,7 +7486,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1090786496"/>
+        <c:crossAx val="1171682832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7584,7 +7550,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7763,11 +7728,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1090743520"/>
-        <c:axId val="1090746912"/>
+        <c:axId val="1396840288"/>
+        <c:axId val="1297141696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1090743520"/>
+        <c:axId val="1396840288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7813,7 +7778,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7879,12 +7843,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1090746912"/>
+        <c:crossAx val="1297141696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1090746912"/>
+        <c:axId val="1297141696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7940,7 +7904,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1090743520"/>
+        <c:crossAx val="1396840288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8004,7 +7968,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8183,11 +8146,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1090769056"/>
-        <c:axId val="1090772448"/>
+        <c:axId val="1396885968"/>
+        <c:axId val="1397654752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1090769056"/>
+        <c:axId val="1396885968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8233,7 +8196,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8299,12 +8261,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1090772448"/>
+        <c:crossAx val="1397654752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1090772448"/>
+        <c:axId val="1397654752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8360,7 +8322,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1090769056"/>
+        <c:crossAx val="1396885968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8424,7 +8386,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8603,11 +8564,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1090800384"/>
-        <c:axId val="1397246864"/>
+        <c:axId val="1172058432"/>
+        <c:axId val="1172061552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1090800384"/>
+        <c:axId val="1172058432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8653,7 +8614,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8719,12 +8679,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1397246864"/>
+        <c:crossAx val="1172061552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1397246864"/>
+        <c:axId val="1172061552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8780,7 +8740,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1090800384"/>
+        <c:crossAx val="1172058432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8844,7 +8804,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9023,11 +8982,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1028553504"/>
-        <c:axId val="1028453984"/>
+        <c:axId val="1171803728"/>
+        <c:axId val="1171806848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1028553504"/>
+        <c:axId val="1171803728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9073,7 +9032,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9139,12 +9097,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1028453984"/>
+        <c:crossAx val="1171806848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1028453984"/>
+        <c:axId val="1171806848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9200,7 +9158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1028553504"/>
+        <c:crossAx val="1171803728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9264,7 +9222,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9443,11 +9400,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1028330624"/>
-        <c:axId val="1091433168"/>
+        <c:axId val="1171827680"/>
+        <c:axId val="1171831072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1028330624"/>
+        <c:axId val="1171827680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9493,7 +9450,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9559,12 +9515,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1091433168"/>
+        <c:crossAx val="1171831072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1091433168"/>
+        <c:axId val="1171831072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9620,7 +9576,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1028330624"/>
+        <c:crossAx val="1171827680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9684,7 +9640,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9863,11 +9818,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1296854192"/>
-        <c:axId val="1440114944"/>
+        <c:axId val="1297844864"/>
+        <c:axId val="1396953520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1296854192"/>
+        <c:axId val="1297844864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9913,7 +9868,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9979,12 +9933,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440114944"/>
+        <c:crossAx val="1396953520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1440114944"/>
+        <c:axId val="1396953520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10040,7 +9994,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1296854192"/>
+        <c:crossAx val="1297844864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10104,7 +10058,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10283,11 +10236,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1028209728"/>
-        <c:axId val="1028528512"/>
+        <c:axId val="1172115808"/>
+        <c:axId val="1172119200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1028209728"/>
+        <c:axId val="1172115808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10333,7 +10286,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10399,12 +10351,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1028528512"/>
+        <c:crossAx val="1172119200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1028528512"/>
+        <c:axId val="1172119200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10460,7 +10412,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1028209728"/>
+        <c:crossAx val="1172115808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10524,7 +10476,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10703,11 +10654,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1505086912"/>
-        <c:axId val="1505090032"/>
+        <c:axId val="1172140016"/>
+        <c:axId val="1172143408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1505086912"/>
+        <c:axId val="1172140016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10753,7 +10704,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10819,12 +10769,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505090032"/>
+        <c:crossAx val="1172143408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1505090032"/>
+        <c:axId val="1172143408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10880,7 +10830,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505086912"/>
+        <c:crossAx val="1172140016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10944,7 +10894,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11123,11 +11072,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1029168480"/>
-        <c:axId val="1505666032"/>
+        <c:axId val="1171725216"/>
+        <c:axId val="1171728608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1029168480"/>
+        <c:axId val="1171725216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11173,7 +11122,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11239,12 +11187,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505666032"/>
+        <c:crossAx val="1171728608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1505666032"/>
+        <c:axId val="1171728608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11300,7 +11248,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1029168480"/>
+        <c:crossAx val="1171725216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11364,7 +11312,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11543,11 +11490,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1093249760"/>
-        <c:axId val="1093253152"/>
+        <c:axId val="1171264512"/>
+        <c:axId val="1171267904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1093249760"/>
+        <c:axId val="1171264512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11593,7 +11540,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11659,12 +11605,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1093253152"/>
+        <c:crossAx val="1171267904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1093253152"/>
+        <c:axId val="1171267904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11720,7 +11666,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1093249760"/>
+        <c:crossAx val="1171264512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11784,7 +11730,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11963,11 +11908,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1029647104"/>
-        <c:axId val="1504718816"/>
+        <c:axId val="1171288992"/>
+        <c:axId val="1171292384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1029647104"/>
+        <c:axId val="1171288992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12013,7 +11958,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12079,12 +12023,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1504718816"/>
+        <c:crossAx val="1171292384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1504718816"/>
+        <c:axId val="1171292384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12140,7 +12084,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1029647104"/>
+        <c:crossAx val="1171288992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12204,7 +12148,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12383,11 +12326,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1093044752"/>
-        <c:axId val="1505282912"/>
+        <c:axId val="1171312704"/>
+        <c:axId val="1171316096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1093044752"/>
+        <c:axId val="1171312704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12433,7 +12376,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12499,12 +12441,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505282912"/>
+        <c:crossAx val="1171316096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1505282912"/>
+        <c:axId val="1171316096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12560,7 +12502,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1093044752"/>
+        <c:crossAx val="1171312704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12624,7 +12566,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12803,11 +12744,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1505064976"/>
-        <c:axId val="1505181712"/>
+        <c:axId val="1171336496"/>
+        <c:axId val="1171339888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1505064976"/>
+        <c:axId val="1171336496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12853,7 +12794,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12919,12 +12859,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505181712"/>
+        <c:crossAx val="1171339888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1505181712"/>
+        <c:axId val="1171339888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12980,7 +12920,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505064976"/>
+        <c:crossAx val="1171336496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13044,7 +12984,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13223,11 +13162,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1505339424"/>
-        <c:axId val="1505342816"/>
+        <c:axId val="1171360416"/>
+        <c:axId val="1171363808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1505339424"/>
+        <c:axId val="1171360416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13273,7 +13212,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -13339,12 +13277,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505342816"/>
+        <c:crossAx val="1171363808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1505342816"/>
+        <c:axId val="1171363808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13400,7 +13338,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505339424"/>
+        <c:crossAx val="1171360416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13464,7 +13402,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13643,11 +13580,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1505118064"/>
-        <c:axId val="1505121184"/>
+        <c:axId val="1171384176"/>
+        <c:axId val="1171387568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1505118064"/>
+        <c:axId val="1171384176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13693,7 +13630,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -13759,12 +13695,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505121184"/>
+        <c:crossAx val="1171387568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1505121184"/>
+        <c:axId val="1171387568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13820,7 +13756,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505118064"/>
+        <c:crossAx val="1171384176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13884,7 +13820,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14063,11 +13998,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1505528368"/>
-        <c:axId val="1505575712"/>
+        <c:axId val="1171407968"/>
+        <c:axId val="1171411360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1505528368"/>
+        <c:axId val="1171407968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14113,7 +14048,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14179,12 +14113,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505575712"/>
+        <c:crossAx val="1171411360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1505575712"/>
+        <c:axId val="1171411360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14240,7 +14174,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505528368"/>
+        <c:crossAx val="1171407968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14304,7 +14238,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14483,11 +14416,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1029625328"/>
-        <c:axId val="1029628448"/>
+        <c:axId val="1396818784"/>
+        <c:axId val="1297919568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1029625328"/>
+        <c:axId val="1396818784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14533,7 +14466,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14599,12 +14531,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1029628448"/>
+        <c:crossAx val="1297919568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1029628448"/>
+        <c:axId val="1297919568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14660,7 +14592,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1029625328"/>
+        <c:crossAx val="1396818784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14724,7 +14656,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14903,11 +14834,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1093564672"/>
-        <c:axId val="1506206256"/>
+        <c:axId val="1171431760"/>
+        <c:axId val="1171435152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1093564672"/>
+        <c:axId val="1171431760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14953,7 +14884,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15019,12 +14949,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1506206256"/>
+        <c:crossAx val="1171435152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1506206256"/>
+        <c:axId val="1171435152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15080,7 +15010,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1093564672"/>
+        <c:crossAx val="1171431760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15144,7 +15074,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15323,11 +15252,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1425093104"/>
-        <c:axId val="1118371760"/>
+        <c:axId val="1171455552"/>
+        <c:axId val="1171458944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1425093104"/>
+        <c:axId val="1171455552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15373,7 +15302,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15439,12 +15367,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1118371760"/>
+        <c:crossAx val="1171458944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1118371760"/>
+        <c:axId val="1171458944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15500,7 +15428,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1425093104"/>
+        <c:crossAx val="1171455552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15564,7 +15492,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15743,11 +15670,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1031214272"/>
-        <c:axId val="1031153600"/>
+        <c:axId val="1171479264"/>
+        <c:axId val="1171482656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1031214272"/>
+        <c:axId val="1171479264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15793,7 +15720,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15859,12 +15785,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031153600"/>
+        <c:crossAx val="1171482656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1031153600"/>
+        <c:axId val="1171482656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15920,7 +15846,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031214272"/>
+        <c:crossAx val="1171479264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15984,7 +15910,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16163,11 +16088,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1118347664"/>
-        <c:axId val="1118351056"/>
+        <c:axId val="1171503056"/>
+        <c:axId val="1171506448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1118347664"/>
+        <c:axId val="1171503056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16213,7 +16138,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16279,12 +16203,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1118351056"/>
+        <c:crossAx val="1171506448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1118351056"/>
+        <c:axId val="1171506448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16340,7 +16264,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1118347664"/>
+        <c:crossAx val="1171503056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16404,7 +16328,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16583,11 +16506,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1031126256"/>
-        <c:axId val="1031092944"/>
+        <c:axId val="1171526848"/>
+        <c:axId val="1171530240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1031126256"/>
+        <c:axId val="1171526848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16633,7 +16556,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16699,12 +16621,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031092944"/>
+        <c:crossAx val="1171530240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1031092944"/>
+        <c:axId val="1171530240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16760,7 +16682,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031126256"/>
+        <c:crossAx val="1171526848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16824,7 +16746,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17003,11 +16924,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1031129632"/>
-        <c:axId val="1031133024"/>
+        <c:axId val="1171550560"/>
+        <c:axId val="1171553952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1031129632"/>
+        <c:axId val="1171550560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17053,7 +16974,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -17119,12 +17039,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031133024"/>
+        <c:crossAx val="1171553952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1031133024"/>
+        <c:axId val="1171553952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17180,7 +17100,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031129632"/>
+        <c:crossAx val="1171550560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17244,7 +17164,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17423,11 +17342,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1031067472"/>
-        <c:axId val="1031058544"/>
+        <c:axId val="1171574352"/>
+        <c:axId val="1171577744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1031067472"/>
+        <c:axId val="1171574352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17473,7 +17392,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -17539,12 +17457,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031058544"/>
+        <c:crossAx val="1171577744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1031058544"/>
+        <c:axId val="1171577744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17600,7 +17518,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031067472"/>
+        <c:crossAx val="1171574352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17664,7 +17582,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17843,11 +17760,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1031028240"/>
-        <c:axId val="1031031360"/>
+        <c:axId val="1171598192"/>
+        <c:axId val="1171601584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1031028240"/>
+        <c:axId val="1171598192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17893,7 +17810,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -17959,12 +17875,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031031360"/>
+        <c:crossAx val="1171601584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1031031360"/>
+        <c:axId val="1171601584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18020,7 +17936,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031028240"/>
+        <c:crossAx val="1171598192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18084,7 +18000,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18263,11 +18178,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1031004896"/>
-        <c:axId val="1030996896"/>
+        <c:axId val="1171621952"/>
+        <c:axId val="1171625344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1031004896"/>
+        <c:axId val="1171621952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18313,7 +18228,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -18379,12 +18293,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1030996896"/>
+        <c:crossAx val="1171625344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1030996896"/>
+        <c:axId val="1171625344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18440,7 +18354,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031004896"/>
+        <c:crossAx val="1171621952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18504,7 +18418,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18683,11 +18596,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1030983328"/>
-        <c:axId val="1030966480"/>
+        <c:axId val="1171646432"/>
+        <c:axId val="1171649824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1030983328"/>
+        <c:axId val="1171646432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18733,7 +18646,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -18799,12 +18711,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1030966480"/>
+        <c:crossAx val="1171649824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1030966480"/>
+        <c:axId val="1171649824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18860,7 +18772,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1030983328"/>
+        <c:crossAx val="1171646432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18924,7 +18836,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19103,11 +19014,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1028901056"/>
-        <c:axId val="1028657616"/>
+        <c:axId val="1395884672"/>
+        <c:axId val="1396103760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1028901056"/>
+        <c:axId val="1395884672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19153,7 +19064,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -19219,12 +19129,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1028657616"/>
+        <c:crossAx val="1396103760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1028657616"/>
+        <c:axId val="1396103760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19280,7 +19190,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1028901056"/>
+        <c:crossAx val="1395884672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -19344,7 +19254,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19523,11 +19432,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1030949248"/>
-        <c:axId val="1030941712"/>
+        <c:axId val="1171670144"/>
+        <c:axId val="1171673536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1030949248"/>
+        <c:axId val="1171670144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19573,7 +19482,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -19639,12 +19547,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1030941712"/>
+        <c:crossAx val="1171673536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1030941712"/>
+        <c:axId val="1171673536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19700,7 +19608,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1030949248"/>
+        <c:crossAx val="1171670144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -19764,7 +19672,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19943,11 +19850,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1029608816"/>
-        <c:axId val="1505866544"/>
+        <c:axId val="1396160224"/>
+        <c:axId val="1396163616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1029608816"/>
+        <c:axId val="1396160224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19993,7 +19900,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -20059,12 +19965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505866544"/>
+        <c:crossAx val="1396163616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1505866544"/>
+        <c:axId val="1396163616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20120,7 +20026,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1029608816"/>
+        <c:crossAx val="1396160224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -20184,7 +20090,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20363,11 +20268,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1441705280"/>
-        <c:axId val="1441708432"/>
+        <c:axId val="1396122224"/>
+        <c:axId val="1396128352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1441705280"/>
+        <c:axId val="1396122224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20413,7 +20318,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -20479,12 +20383,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1441708432"/>
+        <c:crossAx val="1396128352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1441708432"/>
+        <c:axId val="1396128352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20540,7 +20444,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1441705280"/>
+        <c:crossAx val="1396122224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -20604,7 +20508,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20783,11 +20686,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1440350976"/>
-        <c:axId val="1440359456"/>
+        <c:axId val="1396027616"/>
+        <c:axId val="1436383440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1440350976"/>
+        <c:axId val="1396027616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20833,7 +20736,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -20899,12 +20801,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440359456"/>
+        <c:crossAx val="1436383440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1440359456"/>
+        <c:axId val="1436383440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20960,7 +20862,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440350976"/>
+        <c:crossAx val="1396027616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -21024,7 +20926,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21203,11 +21104,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1438533952"/>
-        <c:axId val="1438536144"/>
+        <c:axId val="1173369824"/>
+        <c:axId val="1173373216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1438533952"/>
+        <c:axId val="1173369824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21253,7 +21154,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -21319,12 +21219,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1438536144"/>
+        <c:crossAx val="1173373216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1438536144"/>
+        <c:axId val="1173373216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21380,7 +21280,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1438533952"/>
+        <c:crossAx val="1173369824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -51099,7 +50999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
@@ -51511,43 +51411,43 @@
         <v>10</v>
       </c>
       <c r="C13" s="6">
-        <f>AVERAGE(C3:C12)</f>
+        <f t="shared" ref="C13:L13" si="0">AVERAGE(C3:C12)</f>
         <v>8517760</v>
       </c>
       <c r="D13" s="6">
-        <f>AVERAGE(D3:D12)</f>
+        <f t="shared" si="0"/>
         <v>9125811.1999999993</v>
       </c>
       <c r="E13" s="6">
-        <f>AVERAGE(E3:E12)</f>
+        <f t="shared" si="0"/>
         <v>47471027.200000003</v>
       </c>
       <c r="F13" s="6">
-        <f>AVERAGE(F3:F12)</f>
+        <f t="shared" si="0"/>
         <v>44453708.799999997</v>
       </c>
       <c r="G13" s="6">
-        <f>AVERAGE(G3:G12)</f>
+        <f t="shared" si="0"/>
         <v>33533235.199999999</v>
       </c>
       <c r="H13" s="6">
-        <f>AVERAGE(H3:H12)</f>
+        <f t="shared" si="0"/>
         <v>590954598.39999998</v>
       </c>
       <c r="I13" s="6">
-        <f>AVERAGE(I3:I12)</f>
+        <f t="shared" si="0"/>
         <v>37623603.200000003</v>
       </c>
       <c r="J13" s="6">
-        <f>AVERAGE(J3:J12)</f>
+        <f t="shared" si="0"/>
         <v>416817971.19999999</v>
       </c>
       <c r="K13" s="6">
-        <f>AVERAGE(K3:K12)</f>
+        <f t="shared" si="0"/>
         <v>74848768</v>
       </c>
       <c r="L13" s="6">
-        <f>AVERAGE(L3:L12)</f>
+        <f t="shared" si="0"/>
         <v>80605619.200000003</v>
       </c>
     </row>
@@ -51940,43 +51840,43 @@
         <v>10</v>
       </c>
       <c r="C26" s="6">
-        <f>AVERAGE(C16:C25)</f>
+        <f t="shared" ref="C26:L26" si="1">AVERAGE(C16:C25)</f>
         <v>3589443609.5999999</v>
       </c>
       <c r="D26" s="6">
-        <f>AVERAGE(D16:D25)</f>
+        <f t="shared" si="1"/>
         <v>3584624384</v>
       </c>
       <c r="E26" s="6">
-        <f>AVERAGE(E16:E25)</f>
+        <f t="shared" si="1"/>
         <v>40702151372.800003</v>
       </c>
       <c r="F26" s="6">
-        <f>AVERAGE(F16:F25)</f>
+        <f t="shared" si="1"/>
         <v>3966412.7999999998</v>
       </c>
       <c r="G26" s="6">
-        <f>AVERAGE(G16:G25)</f>
+        <f t="shared" si="1"/>
         <v>49789174528</v>
       </c>
       <c r="H26" s="6">
-        <f>AVERAGE(H16:H25)</f>
+        <f t="shared" si="1"/>
         <v>3889894.4</v>
       </c>
       <c r="I26" s="6">
-        <f>AVERAGE(I16:I25)</f>
+        <f t="shared" si="1"/>
         <v>36175382988.800003</v>
       </c>
       <c r="J26" s="6">
-        <f>AVERAGE(J16:J25)</f>
+        <f t="shared" si="1"/>
         <v>11972129280</v>
       </c>
       <c r="K26" s="6">
-        <f>AVERAGE(K16:K25)</f>
+        <f t="shared" si="1"/>
         <v>9595136</v>
       </c>
       <c r="L26" s="6">
-        <f>AVERAGE(L16:L25)</f>
+        <f t="shared" si="1"/>
         <v>288021667200</v>
       </c>
     </row>
@@ -52387,43 +52287,43 @@
         <v>10</v>
       </c>
       <c r="C39" s="6">
-        <f>AVERAGE(C29:C38)</f>
+        <f t="shared" ref="C39:L39" si="2">AVERAGE(C29:C38)</f>
         <v>368955571.19999999</v>
       </c>
       <c r="D39" s="6">
-        <f>AVERAGE(D29:D38)</f>
+        <f t="shared" si="2"/>
         <v>364095641.60000002</v>
       </c>
       <c r="E39" s="6">
-        <f>AVERAGE(E29:E38)</f>
+        <f t="shared" si="2"/>
         <v>465817.59999999998</v>
       </c>
       <c r="F39" s="6">
-        <f>AVERAGE(F29:F38)</f>
+        <f t="shared" si="2"/>
         <v>492108.79999999999</v>
       </c>
       <c r="G39" s="6">
-        <f>AVERAGE(G29:G38)</f>
+        <f t="shared" si="2"/>
         <v>397875.20000000001</v>
       </c>
       <c r="H39" s="6">
-        <f>AVERAGE(H29:H38)</f>
+        <f t="shared" si="2"/>
         <v>359347.20000000001</v>
       </c>
       <c r="I39" s="6">
-        <f>AVERAGE(I29:I38)</f>
+        <f t="shared" si="2"/>
         <v>413952</v>
       </c>
       <c r="J39" s="6">
-        <f>AVERAGE(J29:J38)</f>
+        <f t="shared" si="2"/>
         <v>1207156864</v>
       </c>
       <c r="K39" s="6">
-        <f>AVERAGE(K29:K38)</f>
+        <f t="shared" si="2"/>
         <v>1518643.2</v>
       </c>
       <c r="L39" s="6">
-        <f>AVERAGE(L29:L38)</f>
+        <f t="shared" si="2"/>
         <v>1449267.2</v>
       </c>
     </row>
@@ -52822,43 +52722,43 @@
         <v>10</v>
       </c>
       <c r="C52" s="6">
-        <f>AVERAGE(C42:C51)</f>
+        <f t="shared" ref="C52:L52" si="3">AVERAGE(C42:C51)</f>
         <v>113315200</v>
       </c>
       <c r="D52" s="6">
-        <f>AVERAGE(D42:D51)</f>
+        <f t="shared" si="3"/>
         <v>64307737.600000001</v>
       </c>
       <c r="E52" s="6">
-        <f>AVERAGE(E42:E51)</f>
+        <f t="shared" si="3"/>
         <v>52503782.399999999</v>
       </c>
       <c r="F52" s="6">
-        <f>AVERAGE(F42:F51)</f>
+        <f t="shared" si="3"/>
         <v>26532838.399999999</v>
       </c>
       <c r="G52" s="6">
-        <f>AVERAGE(G42:G51)</f>
+        <f t="shared" si="3"/>
         <v>23113574.399999999</v>
       </c>
       <c r="H52" s="6">
-        <f>AVERAGE(H42:H51)</f>
+        <f t="shared" si="3"/>
         <v>19339955.199999999</v>
       </c>
       <c r="I52" s="6">
-        <f>AVERAGE(I42:I51)</f>
+        <f t="shared" si="3"/>
         <v>21401830.399999999</v>
       </c>
       <c r="J52" s="6">
-        <f>AVERAGE(J42:J51)</f>
+        <f t="shared" si="3"/>
         <v>83968384</v>
       </c>
       <c r="K52" s="6">
-        <f>AVERAGE(K42:K51)</f>
+        <f t="shared" si="3"/>
         <v>11606784</v>
       </c>
       <c r="L52" s="6">
-        <f>AVERAGE(L42:L51)</f>
+        <f t="shared" si="3"/>
         <v>48080128</v>
       </c>
     </row>
@@ -53250,43 +53150,43 @@
         <v>10</v>
       </c>
       <c r="C65" s="6">
-        <f>AVERAGE(C55:C64)</f>
+        <f t="shared" ref="C65:L65" si="4">AVERAGE(C55:C64)</f>
         <v>4080232140.8000002</v>
       </c>
       <c r="D65" s="6">
-        <f>AVERAGE(D55:D64)</f>
+        <f t="shared" si="4"/>
         <v>4022153574.4000001</v>
       </c>
       <c r="E65" s="6">
-        <f>AVERAGE(E55:E64)</f>
+        <f t="shared" si="4"/>
         <v>40802592000</v>
       </c>
       <c r="F65" s="6">
-        <f>AVERAGE(F55:F64)</f>
+        <f t="shared" si="4"/>
         <v>75445068.799999997</v>
       </c>
       <c r="G65" s="6">
-        <f>AVERAGE(G55:G64)</f>
+        <f t="shared" si="4"/>
         <v>49846219212.800003</v>
       </c>
       <c r="H65" s="6">
-        <f>AVERAGE(H55:H64)</f>
+        <f t="shared" si="4"/>
         <v>614543795.20000005</v>
       </c>
       <c r="I65" s="6">
-        <f>AVERAGE(I55:I64)</f>
+        <f t="shared" si="4"/>
         <v>36234822374.400002</v>
       </c>
       <c r="J65" s="6">
-        <f>AVERAGE(J55:J64)</f>
+        <f t="shared" si="4"/>
         <v>13680072499.200001</v>
       </c>
       <c r="K65" s="6">
-        <f>AVERAGE(K55:K64)</f>
+        <f t="shared" si="4"/>
         <v>97569331.200000003</v>
       </c>
       <c r="L65" s="6">
-        <f>AVERAGE(L55:L64)</f>
+        <f t="shared" si="4"/>
         <v>288151802214.40002</v>
       </c>
     </row>

</xml_diff>